<commit_message>
feat: user study analysis
</commit_message>
<xml_diff>
--- a/user-study/analysis.xlsx
+++ b/user-study/analysis.xlsx
@@ -8,15 +8,36 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/henry/Git/GHRVis/user-study/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94BD541D-D343-EA42-9841-645E0D758404}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{060CF28B-0819-F54E-A509-1FFDD1D8C566}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2240" yWindow="4700" windowWidth="31180" windowHeight="22620" activeTab="2" xr2:uid="{88395142-FF8F-6245-9A63-4581E763FBBD}"/>
+    <workbookView xWindow="11260" yWindow="1400" windowWidth="33280" windowHeight="30460" activeTab="2" xr2:uid="{88395142-FF8F-6245-9A63-4581E763FBBD}"/>
   </bookViews>
   <sheets>
     <sheet name="familiarity" sheetId="1" r:id="rId1"/>
     <sheet name="likert" sheetId="2" r:id="rId2"/>
     <sheet name="accuracy" sheetId="3" r:id="rId3"/>
+    <sheet name="participants" sheetId="4" r:id="rId4"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">participants!$A$1</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">participants!$A$2:$A$109</definedName>
+    <definedName name="_xlchart.v1.10" hidden="1">participants!$A:$A</definedName>
+    <definedName name="_xlchart.v1.11" hidden="1">participants!$B:$B</definedName>
+    <definedName name="_xlchart.v1.12" hidden="1">participants!$D:$D</definedName>
+    <definedName name="_xlchart.v1.13" hidden="1">participants!$E:$E</definedName>
+    <definedName name="_xlchart.v1.14" hidden="1">participants!$A:$A</definedName>
+    <definedName name="_xlchart.v1.15" hidden="1">participants!$B:$B</definedName>
+    <definedName name="_xlchart.v1.16" hidden="1">participants!$D:$D</definedName>
+    <definedName name="_xlchart.v1.17" hidden="1">participants!$E:$E</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">participants!$B$1</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">participants!$B$2:$B$109</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">participants!$C$1</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">participants!$C$2:$C$109</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">participants!$D$1</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">participants!$D$2:$D$109</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">participants!$E$1</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">participants!$E$2:$E$109</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -38,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="26">
   <si>
     <t>familiarity</t>
   </si>
@@ -107,6 +128,15 @@
   </si>
   <si>
     <t>Response time without river</t>
+  </si>
+  <si>
+    <t>Correct</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Incorrect</t>
   </si>
 </sst>
 </file>
@@ -192,13 +222,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1348,475 +1379,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Currect Answers</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>accuracy!$B$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>With river</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>accuracy!$A$2:$A$9</c:f>
-              <c:strCache>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>NHS Nottingham and Nottinghamshire CCG</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Oxfordshire</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Northamptonshire</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>South East London</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>NHS Nottingham and Nottinghamshire CCG</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Oxfordshire</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Northamptonshire</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>South East London</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>accuracy!$B$2:$B$9</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-BD4E-A54B-817E-06DB675DAD5A}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>accuracy!$D$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Without river</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent3"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>accuracy!$A$2:$A$9</c:f>
-              <c:strCache>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>NHS Nottingham and Nottinghamshire CCG</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Oxfordshire</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Northamptonshire</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>South East London</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>NHS Nottingham and Nottinghamshire CCG</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Oxfordshire</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Northamptonshire</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>South East London</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>accuracy!$D$2:$D$9</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-BD4E-A54B-817E-06DB675DAD5A}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
-        <c:axId val="846102335"/>
-        <c:axId val="846070335"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="846102335"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="846070335"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="846070335"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="846102335"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2246,6 +1808,2090 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>accuracy!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>With river</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>accuracy!$A$2:$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>NHS Nottingham and Nottinghamshire CCG</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Oxfordshire</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Northamptonshire</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>South East London</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>accuracy!$B$2:$B$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6FA8-2C43-A757-1281655620E6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>accuracy!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Without river</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>accuracy!$A$2:$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>NHS Nottingham and Nottinghamshire CCG</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Oxfordshire</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Northamptonshire</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>South East London</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>accuracy!$D$2:$D$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-6FA8-2C43-A757-1281655620E6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1945967792"/>
+        <c:axId val="491679648"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1945967792"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="491679648"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="491679648"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1945967792"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>RT per Task</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.42893744531933509"/>
+          <c:y val="0"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>participants!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Correct</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>participants!$A$2:$A$109</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="108"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>13</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>participants!$B$2:$B$109</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="108"/>
+                <c:pt idx="0">
+                  <c:v>2.9820000000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16.163</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>115.309</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.57</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.0499999999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.6840000000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.42</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.1020000000000003</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>23.457000000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11.531000000000001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>19.024999999999999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>45.374000000000002</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6.585</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>44.42</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3.4420000000000002</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>20.847999999999999</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>6.9240000000000004</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4.4809999999999999</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>23.218</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>34.5</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>37.802</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>10.84</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>19.914000000000001</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>10.366</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>13.098000000000001</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>4.7779999999999996</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>44.843000000000004</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>37.848999999999997</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>8.7970000000000006</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>37.808</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>17.491</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>4.5670000000000002</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>4.9800000000000004</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>7.8979999999999997</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>7.4349999999999996</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>3.1339999999999999</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>2.5390000000000001</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>12.539</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>7.7119999999999997</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>2.2440000000000002</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>13.417</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>2.2149999999999999</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>14.951000000000001</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>70.567999999999998</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>20.882000000000001</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>9.7509999999999994</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>13.564</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>29.545999999999999</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>56.317999999999998</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>177.423</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>95.218000000000004</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>6.093</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>51.622999999999998</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>7.5419999999999998</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>16.23</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>7.4710000000000001</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>9.9580000000000002</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>4.46</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>15.098000000000001</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>4.3819999999999997</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>4.9290000000000003</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>5.49</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>3.0640000000000001</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>15.278</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>3.246</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>12.706</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>2.056</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>3.31</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>2.081</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>3.0249999999999999</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>2.16</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>4.4619999999999997</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>4.4649999999999999</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>6.5869999999999997</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>8.1999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>3.7330000000000001</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>2.391</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>2.3889999999999998</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>4.8360000000000003</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>7.4279999999999999</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>7.9569999999999999</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>2.722</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>3.4980000000000002</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>3.8090000000000002</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>3.74</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>1.9750000000000001</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>7.8310000000000004</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>3.7970000000000002</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>3.149</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>7.931</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>5.7409999999999997</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>7.4279999999999999</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>2.8090000000000002</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>4.492</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>4.9210000000000003</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>8.3450000000000006</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>5.6319999999999997</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>4.3559999999999999</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>2.9569999999999999</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>3.74</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>3.1680000000000001</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>3.4980000000000002</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>2.9569999999999999</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>3.9740000000000002</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>2.9750000000000001</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>3.258</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>3.6539999999999999</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>1.9750000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0A6C-C543-BDAE-37A4BFEA9262}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>participants!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Incorrect</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="x"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>participants!$A$2:$A$109</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="108"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>13</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>participants!$E$2:$E$109</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="108"/>
+                <c:pt idx="0">
+                  <c:v>29.285</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>34.735999999999997</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>18.952999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>29.292999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16.452999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.1429999999999998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>16.79</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.7939999999999996</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>48.192999999999998</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>42.709000000000003</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>40.526000000000003</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>35.423000000000002</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>37.511000000000003</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>126.413</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>20.125</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>18.495999999999999</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>46.877000000000002</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>5.0309999999999997</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>11.872999999999999</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>72.933999999999997</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>18.350000000000001</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>52.613</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>159.29300000000001</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>17.29</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>23.704999999999998</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>14.257</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>35.000999999999998</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>42.924999999999997</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>13.756</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>17.835999999999999</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>45.162999999999997</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>50.055999999999997</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>11.977</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>10.231</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>12.146000000000001</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>12.12</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>16.434999999999999</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>19.548999999999999</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>11.272</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>8.67</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>58.634999999999998</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>120.66800000000001</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>135.00200000000001</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>47.816000000000003</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>174.55099999999999</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>12.374000000000001</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>12.237</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>18.920000000000002</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>29.324000000000002</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>42.280999999999999</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>20.018999999999998</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>40.811</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>11.802</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>4.407</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>17.327999999999999</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>5.75</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>9.7729999999999997</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>43.006999999999998</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>11.407</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>7.327</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>9.7880000000000003</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>36.148000000000003</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>6.6210000000000004</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>4.4279999999999999</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>10.981999999999999</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>5.6849999999999996</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>9.9260000000000002</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>4.68</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>5.7130000000000001</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>10.555</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>2.8959999999999999</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>5.085</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>4.3559999999999999</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>10.082000000000001</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>5.4</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>6.4669999999999996</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>6.327</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>6.69</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>7.343</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>9.3239999999999998</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>4.43</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>9.84</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>4.3940000000000001</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>5.5410000000000004</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>4.8</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>4.0090000000000003</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>4.327</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>7.3810000000000002</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>7.7439999999999998</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>6.4870000000000001</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>10.198</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>6.8470000000000004</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>6.2370000000000001</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>8.3000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>3.11</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>4.3029999999999999</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>4.5609999999999999</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>4.4139999999999997</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>3.8159999999999998</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>3.4020000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-0A6C-C543-BDAE-37A4BFEA9262}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="458726032"/>
+        <c:axId val="458727680"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="458726032"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="16"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="458727680"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="1"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="458727680"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="458726032"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -2406,6 +4052,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -4399,6 +6085,522 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -4505,22 +6707,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
+      <xdr:colOff>1089522</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>96398</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>774700</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>104507</xdr:colOff>
+      <xdr:row>78</xdr:row>
+      <xdr:rowOff>45598</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
+        <xdr:cNvPr id="4" name="Chart 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FCA2DA8D-A592-77A7-FD3D-8A101F45E1A7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D9C396FD-BCDD-602B-BD30-A7DDC5A07937}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4541,22 +6743,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>171450</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
+      <xdr:colOff>1098550</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>12700</xdr:colOff>
-      <xdr:row>78</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>584200</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3">
+        <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D9C396FD-BCDD-602B-BD30-A7DDC5A07937}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B308CD5C-3B4B-188F-DC78-AED49ECAE710}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4569,6 +6771,47 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>390864</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>82237</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>818253</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>156744</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6FFFFE43-DFD9-581A-77E5-B2C060982E0E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -5104,8 +7347,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D30E0A9B-B46B-6345-BB06-BCE9FD23E4DB}">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="M50" sqref="M50"/>
+    <sheetView tabSelected="1" zoomScale="83" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5139,13 +7382,13 @@
         <v>15</v>
       </c>
       <c r="B2" s="4">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="C2" s="4">
         <v>6.7690000000000001</v>
       </c>
       <c r="D2" s="4">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="E2" s="4">
         <v>8.7102307692307601</v>
@@ -5157,13 +7400,13 @@
         <v>16</v>
       </c>
       <c r="B3" s="4">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="C3" s="4">
         <v>13.4124615384615</v>
       </c>
       <c r="D3" s="4">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="E3" s="4">
         <v>27.076076923076901</v>
@@ -5175,13 +7418,13 @@
         <v>17</v>
       </c>
       <c r="B4" s="4">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="C4" s="4">
         <v>17.663615384615301</v>
       </c>
       <c r="D4" s="4">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E4" s="4">
         <v>31.492538461538398</v>
@@ -5193,13 +7436,13 @@
         <v>18</v>
       </c>
       <c r="B5" s="4">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C5" s="4">
         <v>30.4855384615384</v>
       </c>
       <c r="D5" s="4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E5" s="4">
         <v>37.515846153846098</v>
@@ -5284,6 +7527,1506 @@
       </c>
       <c r="F9" s="4" t="s">
         <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CEA505E-BD54-7843-8B5C-748559B3F965}">
+  <dimension ref="A1:E109"/>
+  <sheetViews>
+    <sheetView zoomScale="109" workbookViewId="0">
+      <selection activeCell="K35" sqref="K35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="6"/>
+    <col min="2" max="2" width="22.5" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" style="6"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="6">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>2.9820000000000002</v>
+      </c>
+      <c r="D2" s="6">
+        <v>2</v>
+      </c>
+      <c r="E2">
+        <v>29.285</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="6">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>16.163</v>
+      </c>
+      <c r="D3" s="6">
+        <v>6</v>
+      </c>
+      <c r="E3">
+        <v>34.735999999999997</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="6">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>115.309</v>
+      </c>
+      <c r="D4" s="6">
+        <v>7</v>
+      </c>
+      <c r="E4">
+        <v>18.952999999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="6">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>2.57</v>
+      </c>
+      <c r="D5" s="6">
+        <v>8</v>
+      </c>
+      <c r="E5">
+        <v>29.292999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="6">
+        <v>9</v>
+      </c>
+      <c r="B6">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="D6" s="6">
+        <v>10</v>
+      </c>
+      <c r="E6">
+        <v>16.452999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="6">
+        <v>11</v>
+      </c>
+      <c r="B7">
+        <v>6.6840000000000002</v>
+      </c>
+      <c r="D7" s="6">
+        <v>12</v>
+      </c>
+      <c r="E7">
+        <v>7.1429999999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="6">
+        <v>13</v>
+      </c>
+      <c r="B8">
+        <v>2.42</v>
+      </c>
+      <c r="D8" s="6">
+        <v>14</v>
+      </c>
+      <c r="E8">
+        <v>16.79</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="6">
+        <v>15</v>
+      </c>
+      <c r="B9">
+        <v>5.1020000000000003</v>
+      </c>
+      <c r="D9" s="6">
+        <v>2</v>
+      </c>
+      <c r="E9">
+        <v>4.7939999999999996</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="6">
+        <v>16</v>
+      </c>
+      <c r="B10">
+        <v>23.457000000000001</v>
+      </c>
+      <c r="D10" s="6">
+        <v>6</v>
+      </c>
+      <c r="E10">
+        <v>48.192999999999998</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="6">
+        <v>1</v>
+      </c>
+      <c r="B11">
+        <v>11.531000000000001</v>
+      </c>
+      <c r="D11" s="6">
+        <v>8</v>
+      </c>
+      <c r="E11">
+        <v>42.709000000000003</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="6">
+        <v>3</v>
+      </c>
+      <c r="B12">
+        <v>19.024999999999999</v>
+      </c>
+      <c r="D12" s="6">
+        <v>12</v>
+      </c>
+      <c r="E12">
+        <v>40.526000000000003</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="6">
+        <v>4</v>
+      </c>
+      <c r="B13">
+        <v>45.374000000000002</v>
+      </c>
+      <c r="D13" s="6">
+        <v>14</v>
+      </c>
+      <c r="E13">
+        <v>35.423000000000002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="6">
+        <v>5</v>
+      </c>
+      <c r="B14">
+        <v>6.585</v>
+      </c>
+      <c r="D14" s="6">
+        <v>15</v>
+      </c>
+      <c r="E14">
+        <v>37.511000000000003</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="6">
+        <v>7</v>
+      </c>
+      <c r="B15">
+        <v>44.42</v>
+      </c>
+      <c r="D15" s="6">
+        <v>16</v>
+      </c>
+      <c r="E15">
+        <v>126.413</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="6">
+        <v>9</v>
+      </c>
+      <c r="B16">
+        <v>3.4420000000000002</v>
+      </c>
+      <c r="D16" s="6">
+        <v>2</v>
+      </c>
+      <c r="E16">
+        <v>20.125</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="6">
+        <v>10</v>
+      </c>
+      <c r="B17">
+        <v>20.847999999999999</v>
+      </c>
+      <c r="D17" s="6">
+        <v>7</v>
+      </c>
+      <c r="E17">
+        <v>18.495999999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="6">
+        <v>11</v>
+      </c>
+      <c r="B18">
+        <v>6.9240000000000004</v>
+      </c>
+      <c r="D18" s="6">
+        <v>8</v>
+      </c>
+      <c r="E18">
+        <v>46.877000000000002</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="6">
+        <v>13</v>
+      </c>
+      <c r="B19">
+        <v>4.4809999999999999</v>
+      </c>
+      <c r="D19" s="6">
+        <v>10</v>
+      </c>
+      <c r="E19">
+        <v>5.0309999999999997</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="6">
+        <v>1</v>
+      </c>
+      <c r="B20">
+        <v>23.218</v>
+      </c>
+      <c r="D20" s="6">
+        <v>11</v>
+      </c>
+      <c r="E20">
+        <v>11.872999999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="6">
+        <v>3</v>
+      </c>
+      <c r="B21">
+        <v>34.5</v>
+      </c>
+      <c r="D21" s="6">
+        <v>12</v>
+      </c>
+      <c r="E21">
+        <v>72.933999999999997</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="6">
+        <v>4</v>
+      </c>
+      <c r="B22">
+        <v>37.802</v>
+      </c>
+      <c r="D22" s="6">
+        <v>14</v>
+      </c>
+      <c r="E22">
+        <v>18.350000000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="6">
+        <v>5</v>
+      </c>
+      <c r="B23">
+        <v>10.84</v>
+      </c>
+      <c r="D23" s="6">
+        <v>15</v>
+      </c>
+      <c r="E23">
+        <v>52.613</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="6">
+        <v>6</v>
+      </c>
+      <c r="B24">
+        <v>19.914000000000001</v>
+      </c>
+      <c r="D24" s="6">
+        <v>16</v>
+      </c>
+      <c r="E24">
+        <v>159.29300000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="6">
+        <v>9</v>
+      </c>
+      <c r="B25">
+        <v>10.366</v>
+      </c>
+      <c r="D25" s="6">
+        <v>2</v>
+      </c>
+      <c r="E25">
+        <v>17.29</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" s="6">
+        <v>13</v>
+      </c>
+      <c r="B26">
+        <v>13.098000000000001</v>
+      </c>
+      <c r="D26" s="6">
+        <v>7</v>
+      </c>
+      <c r="E26">
+        <v>23.704999999999998</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" s="6">
+        <v>1</v>
+      </c>
+      <c r="B27">
+        <v>4.7779999999999996</v>
+      </c>
+      <c r="D27" s="6">
+        <v>11</v>
+      </c>
+      <c r="E27">
+        <v>14.257</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" s="6">
+        <v>3</v>
+      </c>
+      <c r="B28">
+        <v>44.843000000000004</v>
+      </c>
+      <c r="D28" s="6">
+        <v>12</v>
+      </c>
+      <c r="E28">
+        <v>35.000999999999998</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" s="6">
+        <v>4</v>
+      </c>
+      <c r="B29">
+        <v>37.848999999999997</v>
+      </c>
+      <c r="D29" s="6">
+        <v>14</v>
+      </c>
+      <c r="E29">
+        <v>42.924999999999997</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" s="6">
+        <v>5</v>
+      </c>
+      <c r="B30">
+        <v>8.7970000000000006</v>
+      </c>
+      <c r="D30" s="6">
+        <v>15</v>
+      </c>
+      <c r="E30">
+        <v>13.756</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" s="6">
+        <v>6</v>
+      </c>
+      <c r="B31">
+        <v>37.808</v>
+      </c>
+      <c r="D31" s="6">
+        <v>16</v>
+      </c>
+      <c r="E31">
+        <v>17.835999999999999</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" s="6">
+        <v>8</v>
+      </c>
+      <c r="B32">
+        <v>17.491</v>
+      </c>
+      <c r="D32" s="6">
+        <v>2</v>
+      </c>
+      <c r="E32">
+        <v>45.162999999999997</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" s="6">
+        <v>9</v>
+      </c>
+      <c r="B33">
+        <v>4.5670000000000002</v>
+      </c>
+      <c r="D33" s="6">
+        <v>3</v>
+      </c>
+      <c r="E33">
+        <v>50.055999999999997</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" s="6">
+        <v>10</v>
+      </c>
+      <c r="B34">
+        <v>4.9800000000000004</v>
+      </c>
+      <c r="D34" s="6">
+        <v>4</v>
+      </c>
+      <c r="E34">
+        <v>11.977</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" s="6">
+        <v>13</v>
+      </c>
+      <c r="B35">
+        <v>7.8979999999999997</v>
+      </c>
+      <c r="D35" s="6">
+        <v>6</v>
+      </c>
+      <c r="E35">
+        <v>10.231</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" s="6">
+        <v>1</v>
+      </c>
+      <c r="B36">
+        <v>7.4349999999999996</v>
+      </c>
+      <c r="D36" s="6">
+        <v>7</v>
+      </c>
+      <c r="E36">
+        <v>12.146000000000001</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" s="6">
+        <v>5</v>
+      </c>
+      <c r="B37">
+        <v>3.1339999999999999</v>
+      </c>
+      <c r="D37" s="6">
+        <v>8</v>
+      </c>
+      <c r="E37">
+        <v>12.12</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" s="6">
+        <v>9</v>
+      </c>
+      <c r="B38">
+        <v>2.5390000000000001</v>
+      </c>
+      <c r="D38" s="6">
+        <v>12</v>
+      </c>
+      <c r="E38">
+        <v>16.434999999999999</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39" s="6">
+        <v>10</v>
+      </c>
+      <c r="B39">
+        <v>12.539</v>
+      </c>
+      <c r="D39" s="6">
+        <v>15</v>
+      </c>
+      <c r="E39">
+        <v>19.548999999999999</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40" s="6">
+        <v>11</v>
+      </c>
+      <c r="B40">
+        <v>7.7119999999999997</v>
+      </c>
+      <c r="D40" s="6">
+        <v>16</v>
+      </c>
+      <c r="E40">
+        <v>11.272</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41" s="6">
+        <v>13</v>
+      </c>
+      <c r="B41">
+        <v>2.2440000000000002</v>
+      </c>
+      <c r="D41" s="6">
+        <v>2</v>
+      </c>
+      <c r="E41">
+        <v>8.67</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42" s="6">
+        <v>14</v>
+      </c>
+      <c r="B42">
+        <v>13.417</v>
+      </c>
+      <c r="D42" s="6">
+        <v>4</v>
+      </c>
+      <c r="E42">
+        <v>58.634999999999998</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43" s="6">
+        <v>1</v>
+      </c>
+      <c r="B43">
+        <v>2.2149999999999999</v>
+      </c>
+      <c r="D43" s="6">
+        <v>7</v>
+      </c>
+      <c r="E43">
+        <v>120.66800000000001</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44" s="6">
+        <v>3</v>
+      </c>
+      <c r="B44">
+        <v>14.951000000000001</v>
+      </c>
+      <c r="D44" s="6">
+        <v>8</v>
+      </c>
+      <c r="E44">
+        <v>135.00200000000001</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45" s="6">
+        <v>5</v>
+      </c>
+      <c r="B45">
+        <v>70.567999999999998</v>
+      </c>
+      <c r="D45" s="6">
+        <v>12</v>
+      </c>
+      <c r="E45">
+        <v>47.816000000000003</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46" s="6">
+        <v>6</v>
+      </c>
+      <c r="B46">
+        <v>20.882000000000001</v>
+      </c>
+      <c r="D46" s="6">
+        <v>14</v>
+      </c>
+      <c r="E46">
+        <v>174.55099999999999</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A47" s="6">
+        <v>9</v>
+      </c>
+      <c r="B47">
+        <v>9.7509999999999994</v>
+      </c>
+      <c r="D47" s="6">
+        <v>2</v>
+      </c>
+      <c r="E47">
+        <v>12.374000000000001</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A48" s="6">
+        <v>10</v>
+      </c>
+      <c r="B48">
+        <v>13.564</v>
+      </c>
+      <c r="D48" s="6">
+        <v>3</v>
+      </c>
+      <c r="E48">
+        <v>12.237</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A49" s="6">
+        <v>11</v>
+      </c>
+      <c r="B49">
+        <v>29.545999999999999</v>
+      </c>
+      <c r="D49" s="6">
+        <v>7</v>
+      </c>
+      <c r="E49">
+        <v>18.920000000000002</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A50" s="6">
+        <v>13</v>
+      </c>
+      <c r="B50">
+        <v>56.317999999999998</v>
+      </c>
+      <c r="D50" s="6">
+        <v>8</v>
+      </c>
+      <c r="E50">
+        <v>29.324000000000002</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A51" s="6">
+        <v>15</v>
+      </c>
+      <c r="B51">
+        <v>177.423</v>
+      </c>
+      <c r="D51" s="6">
+        <v>11</v>
+      </c>
+      <c r="E51">
+        <v>42.280999999999999</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A52" s="6">
+        <v>16</v>
+      </c>
+      <c r="B52">
+        <v>95.218000000000004</v>
+      </c>
+      <c r="D52" s="6">
+        <v>12</v>
+      </c>
+      <c r="E52">
+        <v>20.018999999999998</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A53" s="6">
+        <v>1</v>
+      </c>
+      <c r="B53">
+        <v>6.093</v>
+      </c>
+      <c r="D53" s="6">
+        <v>15</v>
+      </c>
+      <c r="E53">
+        <v>40.811</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A54" s="6">
+        <v>4</v>
+      </c>
+      <c r="B54">
+        <v>51.622999999999998</v>
+      </c>
+      <c r="D54" s="6">
+        <v>16</v>
+      </c>
+      <c r="E54">
+        <v>11.802</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A55" s="6">
+        <v>5</v>
+      </c>
+      <c r="B55">
+        <v>7.5419999999999998</v>
+      </c>
+      <c r="D55" s="6">
+        <v>2</v>
+      </c>
+      <c r="E55">
+        <v>4.407</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A56" s="6">
+        <v>6</v>
+      </c>
+      <c r="B56">
+        <v>16.23</v>
+      </c>
+      <c r="D56" s="6">
+        <v>3</v>
+      </c>
+      <c r="E56">
+        <v>17.327999999999999</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A57" s="6">
+        <v>9</v>
+      </c>
+      <c r="B57">
+        <v>7.4710000000000001</v>
+      </c>
+      <c r="D57" s="6">
+        <v>4</v>
+      </c>
+      <c r="E57">
+        <v>5.75</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A58" s="6">
+        <v>10</v>
+      </c>
+      <c r="B58">
+        <v>9.9580000000000002</v>
+      </c>
+      <c r="D58" s="6">
+        <v>7</v>
+      </c>
+      <c r="E58">
+        <v>9.7729999999999997</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A59" s="6">
+        <v>13</v>
+      </c>
+      <c r="B59">
+        <v>4.46</v>
+      </c>
+      <c r="D59" s="6">
+        <v>8</v>
+      </c>
+      <c r="E59">
+        <v>43.006999999999998</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A60" s="6">
+        <v>14</v>
+      </c>
+      <c r="B60">
+        <v>15.098000000000001</v>
+      </c>
+      <c r="D60" s="6">
+        <v>10</v>
+      </c>
+      <c r="E60">
+        <v>11.407</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A61" s="6">
+        <v>1</v>
+      </c>
+      <c r="B61">
+        <v>4.3819999999999997</v>
+      </c>
+      <c r="D61" s="6">
+        <v>11</v>
+      </c>
+      <c r="E61">
+        <v>7.327</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A62" s="6">
+        <v>5</v>
+      </c>
+      <c r="B62">
+        <v>4.9290000000000003</v>
+      </c>
+      <c r="D62" s="6">
+        <v>14</v>
+      </c>
+      <c r="E62">
+        <v>9.7880000000000003</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A63" s="6">
+        <v>6</v>
+      </c>
+      <c r="B63">
+        <v>5.49</v>
+      </c>
+      <c r="D63" s="6">
+        <v>15</v>
+      </c>
+      <c r="E63">
+        <v>36.148000000000003</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A64" s="6">
+        <v>9</v>
+      </c>
+      <c r="B64">
+        <v>3.0640000000000001</v>
+      </c>
+      <c r="D64" s="6">
+        <v>2</v>
+      </c>
+      <c r="E64">
+        <v>6.6210000000000004</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A65" s="6">
+        <v>12</v>
+      </c>
+      <c r="B65">
+        <v>15.278</v>
+      </c>
+      <c r="D65" s="6">
+        <v>3</v>
+      </c>
+      <c r="E65">
+        <v>4.4279999999999999</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A66" s="6">
+        <v>13</v>
+      </c>
+      <c r="B66">
+        <v>3.246</v>
+      </c>
+      <c r="D66" s="6">
+        <v>4</v>
+      </c>
+      <c r="E66">
+        <v>10.981999999999999</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A67" s="6">
+        <v>16</v>
+      </c>
+      <c r="B67">
+        <v>12.706</v>
+      </c>
+      <c r="D67" s="6">
+        <v>6</v>
+      </c>
+      <c r="E67">
+        <v>5.6849999999999996</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A68" s="6">
+        <v>1</v>
+      </c>
+      <c r="B68">
+        <v>2.056</v>
+      </c>
+      <c r="D68" s="6">
+        <v>7</v>
+      </c>
+      <c r="E68">
+        <v>9.9260000000000002</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A69" s="6">
+        <v>5</v>
+      </c>
+      <c r="B69">
+        <v>3.31</v>
+      </c>
+      <c r="D69" s="6">
+        <v>8</v>
+      </c>
+      <c r="E69">
+        <v>4.68</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A70" s="6">
+        <v>9</v>
+      </c>
+      <c r="B70">
+        <v>2.081</v>
+      </c>
+      <c r="D70" s="6">
+        <v>10</v>
+      </c>
+      <c r="E70">
+        <v>5.7130000000000001</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A71" s="6">
+        <v>11</v>
+      </c>
+      <c r="B71">
+        <v>3.0249999999999999</v>
+      </c>
+      <c r="D71" s="6">
+        <v>12</v>
+      </c>
+      <c r="E71">
+        <v>10.555</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A72" s="6">
+        <v>13</v>
+      </c>
+      <c r="B72">
+        <v>2.16</v>
+      </c>
+      <c r="D72" s="6">
+        <v>14</v>
+      </c>
+      <c r="E72">
+        <v>2.8959999999999999</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A73" s="6">
+        <v>1</v>
+      </c>
+      <c r="B73">
+        <v>4.4619999999999997</v>
+      </c>
+      <c r="D73" s="6">
+        <v>15</v>
+      </c>
+      <c r="E73">
+        <v>5.085</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A74" s="6">
+        <v>3</v>
+      </c>
+      <c r="B74">
+        <v>4.4649999999999999</v>
+      </c>
+      <c r="D74" s="6">
+        <v>16</v>
+      </c>
+      <c r="E74">
+        <v>4.3559999999999999</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A75" s="6">
+        <v>4</v>
+      </c>
+      <c r="B75">
+        <v>6.5869999999999997</v>
+      </c>
+      <c r="D75" s="6">
+        <v>2</v>
+      </c>
+      <c r="E75">
+        <v>10.082000000000001</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A76" s="6">
+        <v>5</v>
+      </c>
+      <c r="B76">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="D76" s="6">
+        <v>7</v>
+      </c>
+      <c r="E76">
+        <v>5.4</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A77" s="6">
+        <v>6</v>
+      </c>
+      <c r="B77">
+        <v>3.7330000000000001</v>
+      </c>
+      <c r="D77" s="6">
+        <v>8</v>
+      </c>
+      <c r="E77">
+        <v>6.4669999999999996</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A78" s="6">
+        <v>9</v>
+      </c>
+      <c r="B78">
+        <v>2.391</v>
+      </c>
+      <c r="D78" s="6">
+        <v>12</v>
+      </c>
+      <c r="E78">
+        <v>6.327</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A79" s="6">
+        <v>10</v>
+      </c>
+      <c r="B79">
+        <v>2.3889999999999998</v>
+      </c>
+      <c r="D79" s="6">
+        <v>14</v>
+      </c>
+      <c r="E79">
+        <v>6.69</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A80" s="6">
+        <v>11</v>
+      </c>
+      <c r="B80">
+        <v>4.8360000000000003</v>
+      </c>
+      <c r="D80" s="6">
+        <v>15</v>
+      </c>
+      <c r="E80">
+        <v>7.343</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A81" s="6">
+        <v>13</v>
+      </c>
+      <c r="B81">
+        <v>7.4279999999999999</v>
+      </c>
+      <c r="D81" s="6">
+        <v>16</v>
+      </c>
+      <c r="E81">
+        <v>9.3239999999999998</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A82" s="6">
+        <v>1</v>
+      </c>
+      <c r="B82">
+        <v>7.9569999999999999</v>
+      </c>
+      <c r="D82" s="6">
+        <v>2</v>
+      </c>
+      <c r="E82">
+        <v>4.43</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A83" s="6">
+        <v>3</v>
+      </c>
+      <c r="B83">
+        <v>2.722</v>
+      </c>
+      <c r="D83" s="6">
+        <v>7</v>
+      </c>
+      <c r="E83">
+        <v>9.84</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A84" s="6">
+        <v>4</v>
+      </c>
+      <c r="B84">
+        <v>3.4980000000000002</v>
+      </c>
+      <c r="D84" s="6">
+        <v>8</v>
+      </c>
+      <c r="E84">
+        <v>4.3940000000000001</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A85" s="6">
+        <v>5</v>
+      </c>
+      <c r="B85">
+        <v>3.8090000000000002</v>
+      </c>
+      <c r="D85" s="6">
+        <v>12</v>
+      </c>
+      <c r="E85">
+        <v>5.5410000000000004</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A86" s="6">
+        <v>6</v>
+      </c>
+      <c r="B86">
+        <v>3.74</v>
+      </c>
+      <c r="D86" s="6">
+        <v>14</v>
+      </c>
+      <c r="E86">
+        <v>4.8</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A87" s="6">
+        <v>9</v>
+      </c>
+      <c r="B87">
+        <v>1.9750000000000001</v>
+      </c>
+      <c r="D87" s="6">
+        <v>15</v>
+      </c>
+      <c r="E87">
+        <v>4.0090000000000003</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A88" s="6">
+        <v>10</v>
+      </c>
+      <c r="B88">
+        <v>7.8310000000000004</v>
+      </c>
+      <c r="D88" s="6">
+        <v>16</v>
+      </c>
+      <c r="E88">
+        <v>4.327</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A89" s="6">
+        <v>11</v>
+      </c>
+      <c r="B89">
+        <v>3.7970000000000002</v>
+      </c>
+      <c r="D89" s="6">
+        <v>2</v>
+      </c>
+      <c r="E89">
+        <v>7.3810000000000002</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A90" s="6">
+        <v>13</v>
+      </c>
+      <c r="B90">
+        <v>3.149</v>
+      </c>
+      <c r="D90" s="6">
+        <v>7</v>
+      </c>
+      <c r="E90">
+        <v>7.7439999999999998</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A91" s="6">
+        <v>1</v>
+      </c>
+      <c r="B91">
+        <v>7.931</v>
+      </c>
+      <c r="D91" s="6">
+        <v>8</v>
+      </c>
+      <c r="E91">
+        <v>6.4870000000000001</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A92" s="6">
+        <v>3</v>
+      </c>
+      <c r="B92">
+        <v>5.7409999999999997</v>
+      </c>
+      <c r="D92" s="6">
+        <v>12</v>
+      </c>
+      <c r="E92">
+        <v>10.198</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A93" s="6">
+        <v>4</v>
+      </c>
+      <c r="B93">
+        <v>7.4279999999999999</v>
+      </c>
+      <c r="D93" s="6">
+        <v>14</v>
+      </c>
+      <c r="E93">
+        <v>6.8470000000000004</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A94" s="6">
+        <v>5</v>
+      </c>
+      <c r="B94">
+        <v>2.8090000000000002</v>
+      </c>
+      <c r="D94" s="6">
+        <v>15</v>
+      </c>
+      <c r="E94">
+        <v>6.2370000000000001</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A95" s="6">
+        <v>6</v>
+      </c>
+      <c r="B95">
+        <v>4.492</v>
+      </c>
+      <c r="D95" s="6">
+        <v>16</v>
+      </c>
+      <c r="E95">
+        <v>8.3000000000000007</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A96" s="6">
+        <v>9</v>
+      </c>
+      <c r="B96">
+        <v>4.9210000000000003</v>
+      </c>
+      <c r="D96" s="6">
+        <v>6</v>
+      </c>
+      <c r="E96">
+        <v>3.11</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A97" s="6">
+        <v>10</v>
+      </c>
+      <c r="B97">
+        <v>8.3450000000000006</v>
+      </c>
+      <c r="D97" s="6">
+        <v>8</v>
+      </c>
+      <c r="E97">
+        <v>4.3029999999999999</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A98" s="6">
+        <v>11</v>
+      </c>
+      <c r="B98">
+        <v>5.6319999999999997</v>
+      </c>
+      <c r="D98" s="6">
+        <v>12</v>
+      </c>
+      <c r="E98">
+        <v>4.5609999999999999</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A99" s="6">
+        <v>13</v>
+      </c>
+      <c r="B99">
+        <v>4.3559999999999999</v>
+      </c>
+      <c r="D99" s="6">
+        <v>14</v>
+      </c>
+      <c r="E99">
+        <v>4.4139999999999997</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A100" s="6">
+        <v>1</v>
+      </c>
+      <c r="B100">
+        <v>2.9569999999999999</v>
+      </c>
+      <c r="D100" s="6">
+        <v>15</v>
+      </c>
+      <c r="E100">
+        <v>3.8159999999999998</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A101" s="6">
+        <v>2</v>
+      </c>
+      <c r="B101">
+        <v>3.74</v>
+      </c>
+      <c r="D101" s="6">
+        <v>16</v>
+      </c>
+      <c r="E101">
+        <v>3.4020000000000001</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A102" s="6">
+        <v>3</v>
+      </c>
+      <c r="B102">
+        <v>3.1680000000000001</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A103" s="6">
+        <v>4</v>
+      </c>
+      <c r="B103">
+        <v>3.4980000000000002</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A104" s="6">
+        <v>5</v>
+      </c>
+      <c r="B104">
+        <v>2.9569999999999999</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A105" s="6">
+        <v>7</v>
+      </c>
+      <c r="B105">
+        <v>3.9740000000000002</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A106" s="6">
+        <v>9</v>
+      </c>
+      <c r="B106">
+        <v>2.9750000000000001</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A107" s="6">
+        <v>10</v>
+      </c>
+      <c r="B107">
+        <v>3.258</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A108" s="6">
+        <v>11</v>
+      </c>
+      <c r="B108">
+        <v>3.6539999999999999</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A109" s="6">
+        <v>13</v>
+      </c>
+      <c r="B109">
+        <v>1.9750000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>